<commit_message>
finished feature SBAR + updated scrum
</commit_message>
<xml_diff>
--- a/P13/store/Scrum.xlsx
+++ b/P13/store/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P13/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28CA530-56F0-3C4E-9EC0-0255CE6FA60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A698B808-4F87-7143-9C5E-ABC1CC9C4D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="1020" windowWidth="28800" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="220">
   <si>
     <t>Product Name:</t>
   </si>
@@ -693,6 +693,15 @@
   </si>
   <si>
     <t>Update the "Display" section to make scrollbars always visible</t>
+  </si>
+  <si>
+    <t>Declare and Initialize the statusBar field in the MainWin constructor</t>
+  </si>
+  <si>
+    <t>Create a setStatus method for updating the status bar text.</t>
+  </si>
+  <si>
+    <t>Update listeners to display appropriate status messages.</t>
   </si>
 </sst>
 </file>
@@ -3082,22 +3091,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -3888,8 +3897,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5197,8 +5206,12 @@
       <c r="E53" s="16">
         <v>8</v>
       </c>
-      <c r="F53" s="17"/>
-      <c r="G53" s="17"/>
+      <c r="F53" s="17">
+        <v>6</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>215</v>
+      </c>
       <c r="H53" s="18" t="s">
         <v>79</v>
       </c>
@@ -12052,8 +12065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12160,7 +12173,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -12175,7 +12188,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -12193,7 +12206,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -12211,7 +12224,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -12229,7 +12242,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -12247,7 +12260,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -12269,7 +12282,7 @@
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -12359,34 +12372,52 @@
       </c>
       <c r="F18" s="37"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="35" t="s">
+        <v>127</v>
+      </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="36"/>
+      <c r="D19" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>203</v>
+      </c>
       <c r="F19" s="37"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="35" t="s">
+        <v>127</v>
+      </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="36"/>
+      <c r="D20" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>203</v>
+      </c>
       <c r="F20" s="37"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="35" t="s">
+        <v>127</v>
+      </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="36"/>
+      <c r="D21" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>203</v>
+      </c>
       <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
implementation of feature SPEC + scrum updated
</commit_message>
<xml_diff>
--- a/P13/store/Scrum.xlsx
+++ b/P13/store/Scrum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P13/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92CA9FA-70D4-5347-A924-FD1E8E35E337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470F3DAA-291F-204E-81DC-155FD7FA63DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="540" windowWidth="28800" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="226">
   <si>
     <t>Product Name:</t>
   </si>
@@ -711,6 +711,15 @@
   </si>
   <si>
     <t>Update Computer.addOption + Order.addComputer + Store methods</t>
+  </si>
+  <si>
+    <t>Create the subclass Cpu</t>
+  </si>
+  <si>
+    <t>Update onInsertOptionClick() with radio buttons</t>
+  </si>
+  <si>
+    <t>Save and Restore the specialized Option objects correctly</t>
   </si>
 </sst>
 </file>
@@ -3100,25 +3109,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3906,8 +3915,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5277,8 +5286,12 @@
       <c r="E55" s="16">
         <v>13</v>
       </c>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
+      <c r="F55" s="17">
+        <v>6</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>215</v>
+      </c>
       <c r="H55" s="18" t="s">
         <v>119</v>
       </c>
@@ -12078,8 +12091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12186,7 +12199,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -12201,7 +12214,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -12219,7 +12232,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -12237,7 +12250,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -12255,7 +12268,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -12273,7 +12286,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -12291,7 +12304,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -12313,7 +12326,7 @@
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
@@ -12481,34 +12494,52 @@
       </c>
       <c r="F24" s="37"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="35" t="s">
+        <v>135</v>
+      </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="36"/>
+      <c r="D25" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>185</v>
+      </c>
       <c r="F25" s="37"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="4">
         <v>10</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="35" t="s">
+        <v>135</v>
+      </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="36"/>
+      <c r="D26" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>185</v>
+      </c>
       <c r="F26" s="37"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4">
         <v>11</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="35" t="s">
+        <v>135</v>
+      </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="36"/>
+      <c r="D27" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>185</v>
+      </c>
       <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
finished feature DTAIL + scrum updated
</commit_message>
<xml_diff>
--- a/P13/store/Scrum.xlsx
+++ b/P13/store/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P13/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470F3DAA-291F-204E-81DC-155FD7FA63DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7486936-6BE3-CE47-9B55-264213D65003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="540" windowWidth="28800" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="15880" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="229">
   <si>
     <t>Product Name:</t>
   </si>
@@ -720,6 +720,15 @@
   </si>
   <si>
     <t>Save and Restore the specialized Option objects correctly</t>
+  </si>
+  <si>
+    <t>Update Customer.java with new field + method</t>
+  </si>
+  <si>
+    <t>Update onInsertCustomerClick() to use a FileChooser button</t>
+  </si>
+  <si>
+    <t>Update Mainwin with new menu item + new actionlistener</t>
   </si>
 </sst>
 </file>
@@ -3109,25 +3118,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3915,7 +3924,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A45" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
@@ -5260,7 +5269,9 @@
         <v>21</v>
       </c>
       <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
+      <c r="G54" s="17" t="s">
+        <v>215</v>
+      </c>
       <c r="H54" s="18" t="s">
         <v>119</v>
       </c>
@@ -12091,8 +12102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -12199,7 +12210,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -12214,7 +12225,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -12232,7 +12243,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -12250,7 +12261,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -12268,7 +12279,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -12286,7 +12297,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -12304,7 +12315,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -12326,7 +12337,7 @@
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
@@ -12542,34 +12553,52 @@
       </c>
       <c r="F27" s="37"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="4">
         <v>12</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="35" t="s">
+        <v>131</v>
+      </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="36"/>
+      <c r="D28" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>185</v>
+      </c>
       <c r="F28" s="37"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="4">
         <v>13</v>
       </c>
-      <c r="B29" s="35"/>
+      <c r="B29" s="35" t="s">
+        <v>131</v>
+      </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="36"/>
+      <c r="D29" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>185</v>
+      </c>
       <c r="F29" s="37"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="4">
         <v>14</v>
       </c>
-      <c r="B30" s="35"/>
+      <c r="B30" s="35" t="s">
+        <v>131</v>
+      </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="36"/>
+      <c r="D30" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="E30" s="36" t="s">
+        <v>185</v>
+      </c>
       <c r="F30" s="37"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>